<commit_message>
companies, nationality and sector sorted in 2025
</commit_message>
<xml_diff>
--- a/data/world_countries.xlsx
+++ b/data/world_countries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Drive\ESTUDOS DATA SCIENCE\ie-employment-permit\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\ESTUDOS DATA SCIENCE\ie-employment-permit\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49B6A79-B278-416D-9BBF-A77A01FBA928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86DF7D5-91C2-4556-942E-4A3DBF2F243E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{20B413F9-C870-4C80-9652-07DD00D52B38}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{20B413F9-C870-4C80-9652-07DD00D52B38}"/>
   </bookViews>
   <sheets>
     <sheet name="World" sheetId="1" r:id="rId1"/>
@@ -46,12 +46,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1718" uniqueCount="657">
   <si>
     <t>Country</t>
   </si>
@@ -2013,6 +2016,15 @@
   </si>
   <si>
     <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>Aland Islands</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Christmas Island</t>
   </si>
 </sst>
 </file>
@@ -2382,23 +2394,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0B1C968-BD7A-47B1-B2B0-F423785F7DB9}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F196"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A181" sqref="A181"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2412,7 +2423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2426,7 +2437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2440,7 +2451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2454,7 +2465,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -2468,7 +2479,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2482,7 +2493,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2496,7 +2507,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2510,7 +2521,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2524,7 +2535,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2538,7 +2549,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2552,7 +2563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>39</v>
       </c>
@@ -2566,7 +2577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -2580,7 +2591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2594,7 +2605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -2608,7 +2619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -2622,7 +2633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>54</v>
       </c>
@@ -2636,7 +2647,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>57</v>
       </c>
@@ -2650,7 +2661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>60</v>
       </c>
@@ -2664,7 +2675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -2678,7 +2689,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>66</v>
       </c>
@@ -2692,7 +2703,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -2706,7 +2717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -2720,7 +2731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>75</v>
       </c>
@@ -2734,7 +2745,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>78</v>
       </c>
@@ -2748,7 +2759,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>81</v>
       </c>
@@ -2762,7 +2773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>84</v>
       </c>
@@ -2776,7 +2787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2790,7 +2801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -2804,7 +2815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>93</v>
       </c>
@@ -2818,7 +2829,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>96</v>
       </c>
@@ -2832,7 +2843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>99</v>
       </c>
@@ -2846,7 +2857,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>102</v>
       </c>
@@ -2860,7 +2871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>105</v>
       </c>
@@ -2874,7 +2885,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -2888,7 +2899,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -2902,7 +2913,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>114</v>
       </c>
@@ -2916,7 +2927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -2930,7 +2941,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -2944,7 +2955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>123</v>
       </c>
@@ -2958,7 +2969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>126</v>
       </c>
@@ -2972,7 +2983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>129</v>
       </c>
@@ -2986,7 +2997,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>132</v>
       </c>
@@ -3000,7 +3011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>135</v>
       </c>
@@ -3014,7 +3025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>138</v>
       </c>
@@ -3028,7 +3039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>141</v>
       </c>
@@ -3042,7 +3053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>144</v>
       </c>
@@ -3056,7 +3067,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>147</v>
       </c>
@@ -3070,7 +3081,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -3084,7 +3095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>152</v>
       </c>
@@ -3098,7 +3109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>155</v>
       </c>
@@ -3112,7 +3123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>158</v>
       </c>
@@ -3126,7 +3137,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>161</v>
       </c>
@@ -3140,7 +3151,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>164</v>
       </c>
@@ -3154,7 +3165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>167</v>
       </c>
@@ -3168,7 +3179,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>170</v>
       </c>
@@ -3182,7 +3193,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>173</v>
       </c>
@@ -3196,7 +3207,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>176</v>
       </c>
@@ -3210,7 +3221,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -3224,7 +3235,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>182</v>
       </c>
@@ -3238,7 +3249,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>185</v>
       </c>
@@ -3252,7 +3263,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>188</v>
       </c>
@@ -3266,7 +3277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>191</v>
       </c>
@@ -3280,7 +3291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>194</v>
       </c>
@@ -3294,7 +3305,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>197</v>
       </c>
@@ -3308,7 +3319,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>200</v>
       </c>
@@ -3322,7 +3333,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>203</v>
       </c>
@@ -3336,7 +3347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>206</v>
       </c>
@@ -3350,7 +3361,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>209</v>
       </c>
@@ -3364,7 +3375,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>212</v>
       </c>
@@ -3378,7 +3389,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -3392,7 +3403,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>218</v>
       </c>
@@ -3406,7 +3417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>221</v>
       </c>
@@ -3420,7 +3431,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>224</v>
       </c>
@@ -3434,7 +3445,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>227</v>
       </c>
@@ -3448,7 +3459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>230</v>
       </c>
@@ -3462,7 +3473,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>233</v>
       </c>
@@ -3476,7 +3487,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>236</v>
       </c>
@@ -3490,7 +3501,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>239</v>
       </c>
@@ -3504,7 +3515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="80" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>242</v>
       </c>
@@ -3518,7 +3529,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>245</v>
       </c>
@@ -3532,7 +3543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>248</v>
       </c>
@@ -3546,7 +3557,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="83" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>251</v>
       </c>
@@ -3560,7 +3571,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>254</v>
       </c>
@@ -3574,7 +3585,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>257</v>
       </c>
@@ -3588,7 +3599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>260</v>
       </c>
@@ -3602,7 +3613,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="87" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>263</v>
       </c>
@@ -3616,7 +3627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="88" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>266</v>
       </c>
@@ -3630,7 +3641,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>269</v>
       </c>
@@ -3644,7 +3655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="90" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>272</v>
       </c>
@@ -3658,7 +3669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>275</v>
       </c>
@@ -3672,7 +3683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="92" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>278</v>
       </c>
@@ -3686,7 +3697,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>281</v>
       </c>
@@ -3700,7 +3711,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="94" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>284</v>
       </c>
@@ -3714,7 +3725,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="95" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>287</v>
       </c>
@@ -3728,7 +3739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>290</v>
       </c>
@@ -3742,7 +3753,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>293</v>
       </c>
@@ -3756,7 +3767,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>296</v>
       </c>
@@ -3770,7 +3781,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -3784,7 +3795,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>302</v>
       </c>
@@ -3798,7 +3809,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>305</v>
       </c>
@@ -3812,7 +3823,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>308</v>
       </c>
@@ -3826,7 +3837,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>311</v>
       </c>
@@ -3840,7 +3851,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>314</v>
       </c>
@@ -3855,7 +3866,7 @@
       </c>
       <c r="F104" s="1"/>
     </row>
-    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>317</v>
       </c>
@@ -3870,7 +3881,7 @@
       </c>
       <c r="F105" s="1"/>
     </row>
-    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>320</v>
       </c>
@@ -3885,7 +3896,7 @@
       </c>
       <c r="F106" s="1"/>
     </row>
-    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>323</v>
       </c>
@@ -3900,7 +3911,7 @@
       </c>
       <c r="F107" s="1"/>
     </row>
-    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>326</v>
       </c>
@@ -3915,7 +3926,7 @@
       </c>
       <c r="F108" s="1"/>
     </row>
-    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>329</v>
       </c>
@@ -3930,7 +3941,7 @@
       </c>
       <c r="F109" s="1"/>
     </row>
-    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>332</v>
       </c>
@@ -3945,7 +3956,7 @@
       </c>
       <c r="F110" s="1"/>
     </row>
-    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>335</v>
       </c>
@@ -3960,7 +3971,7 @@
       </c>
       <c r="F111" s="1"/>
     </row>
-    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>338</v>
       </c>
@@ -3975,7 +3986,7 @@
       </c>
       <c r="F112" s="1"/>
     </row>
-    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>341</v>
       </c>
@@ -3990,7 +4001,7 @@
       </c>
       <c r="F113" s="1"/>
     </row>
-    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>344</v>
       </c>
@@ -4005,7 +4016,7 @@
       </c>
       <c r="F114" s="1"/>
     </row>
-    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>347</v>
       </c>
@@ -4020,7 +4031,7 @@
       </c>
       <c r="F115" s="1"/>
     </row>
-    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>349</v>
       </c>
@@ -4035,7 +4046,7 @@
       </c>
       <c r="F116" s="1"/>
     </row>
-    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>352</v>
       </c>
@@ -4050,7 +4061,7 @@
       </c>
       <c r="F117" s="1"/>
     </row>
-    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>355</v>
       </c>
@@ -4065,7 +4076,7 @@
       </c>
       <c r="F118" s="1"/>
     </row>
-    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>358</v>
       </c>
@@ -4080,7 +4091,7 @@
       </c>
       <c r="F119" s="1"/>
     </row>
-    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>361</v>
       </c>
@@ -4095,7 +4106,7 @@
       </c>
       <c r="F120" s="1"/>
     </row>
-    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>364</v>
       </c>
@@ -4110,7 +4121,7 @@
       </c>
       <c r="F121" s="1"/>
     </row>
-    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>367</v>
       </c>
@@ -4125,7 +4136,7 @@
       </c>
       <c r="F122" s="1"/>
     </row>
-    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>370</v>
       </c>
@@ -4140,7 +4151,7 @@
       </c>
       <c r="F123" s="1"/>
     </row>
-    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>373</v>
       </c>
@@ -4155,7 +4166,7 @@
       </c>
       <c r="F124" s="1"/>
     </row>
-    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>376</v>
       </c>
@@ -4170,7 +4181,7 @@
       </c>
       <c r="F125" s="1"/>
     </row>
-    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>379</v>
       </c>
@@ -4185,7 +4196,7 @@
       </c>
       <c r="F126" s="1"/>
     </row>
-    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>382</v>
       </c>
@@ -4200,7 +4211,7 @@
       </c>
       <c r="F127" s="1"/>
     </row>
-    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>385</v>
       </c>
@@ -4215,7 +4226,7 @@
       </c>
       <c r="F128" s="1"/>
     </row>
-    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>388</v>
       </c>
@@ -4230,7 +4241,7 @@
       </c>
       <c r="F129" s="1"/>
     </row>
-    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>391</v>
       </c>
@@ -4245,7 +4256,7 @@
       </c>
       <c r="F130" s="1"/>
     </row>
-    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>394</v>
       </c>
@@ -4260,7 +4271,7 @@
       </c>
       <c r="F131" s="1"/>
     </row>
-    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>397</v>
       </c>
@@ -4275,7 +4286,7 @@
       </c>
       <c r="F132" s="1"/>
     </row>
-    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>400</v>
       </c>
@@ -4290,7 +4301,7 @@
       </c>
       <c r="F133" s="1"/>
     </row>
-    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>403</v>
       </c>
@@ -4305,7 +4316,7 @@
       </c>
       <c r="F134" s="1"/>
     </row>
-    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>406</v>
       </c>
@@ -4320,7 +4331,7 @@
       </c>
       <c r="F135" s="1"/>
     </row>
-    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>409</v>
       </c>
@@ -4335,7 +4346,7 @@
       </c>
       <c r="F136" s="1"/>
     </row>
-    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>412</v>
       </c>
@@ -4350,7 +4361,7 @@
       </c>
       <c r="F137" s="1"/>
     </row>
-    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>415</v>
       </c>
@@ -4365,7 +4376,7 @@
       </c>
       <c r="F138" s="1"/>
     </row>
-    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>418</v>
       </c>
@@ -4380,7 +4391,7 @@
       </c>
       <c r="F139" s="1"/>
     </row>
-    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>421</v>
       </c>
@@ -4395,7 +4406,7 @@
       </c>
       <c r="F140" s="1"/>
     </row>
-    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>424</v>
       </c>
@@ -4410,7 +4421,7 @@
       </c>
       <c r="F141" s="1"/>
     </row>
-    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>427</v>
       </c>
@@ -4425,7 +4436,7 @@
       </c>
       <c r="F142" s="1"/>
     </row>
-    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>430</v>
       </c>
@@ -4440,7 +4451,7 @@
       </c>
       <c r="F143" s="1"/>
     </row>
-    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>433</v>
       </c>
@@ -4455,7 +4466,7 @@
       </c>
       <c r="F144" s="1"/>
     </row>
-    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>436</v>
       </c>
@@ -4470,7 +4481,7 @@
       </c>
       <c r="F145" s="1"/>
     </row>
-    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>439</v>
       </c>
@@ -4485,7 +4496,7 @@
       </c>
       <c r="F146" s="1"/>
     </row>
-    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>442</v>
       </c>
@@ -4499,7 +4510,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>445</v>
       </c>
@@ -4513,7 +4524,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>448</v>
       </c>
@@ -4527,7 +4538,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>450</v>
       </c>
@@ -4541,7 +4552,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>453</v>
       </c>
@@ -4555,7 +4566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>456</v>
       </c>
@@ -4569,7 +4580,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>459</v>
       </c>
@@ -4583,7 +4594,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>462</v>
       </c>
@@ -4597,7 +4608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>465</v>
       </c>
@@ -4611,7 +4622,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>468</v>
       </c>
@@ -4625,7 +4636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>470</v>
       </c>
@@ -4639,7 +4650,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>473</v>
       </c>
@@ -4653,7 +4664,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>476</v>
       </c>
@@ -4667,7 +4678,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>479</v>
       </c>
@@ -4681,7 +4692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="161" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>482</v>
       </c>
@@ -4695,7 +4706,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="162" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>485</v>
       </c>
@@ -4709,7 +4720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="163" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>488</v>
       </c>
@@ -4723,7 +4734,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="164" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>491</v>
       </c>
@@ -4737,7 +4748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="165" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>494</v>
       </c>
@@ -4751,7 +4762,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>497</v>
       </c>
@@ -4765,7 +4776,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="167" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>500</v>
       </c>
@@ -4779,7 +4790,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="168" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>503</v>
       </c>
@@ -4793,7 +4804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="169" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>506</v>
       </c>
@@ -4807,7 +4818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="170" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>509</v>
       </c>
@@ -4821,7 +4832,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="171" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>512</v>
       </c>
@@ -4835,7 +4846,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="172" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -4849,7 +4860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>518</v>
       </c>
@@ -4863,7 +4874,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="174" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -4877,7 +4888,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="175" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>524</v>
       </c>
@@ -4891,7 +4902,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="176" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>527</v>
       </c>
@@ -4905,7 +4916,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="177" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>530</v>
       </c>
@@ -4919,7 +4930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="178" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>533</v>
       </c>
@@ -4933,7 +4944,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="179" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>536</v>
       </c>
@@ -4947,7 +4958,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="180" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>539</v>
       </c>
@@ -4961,7 +4972,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>542</v>
       </c>
@@ -4975,7 +4986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>545</v>
       </c>
@@ -4989,7 +5000,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>548</v>
       </c>
@@ -5003,7 +5014,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="184" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>551</v>
       </c>
@@ -5017,7 +5028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="185" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>554</v>
       </c>
@@ -5031,7 +5042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="186" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>557</v>
       </c>
@@ -5045,7 +5056,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="187" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>560</v>
       </c>
@@ -5059,7 +5070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="188" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>563</v>
       </c>
@@ -5073,7 +5084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="189" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>566</v>
       </c>
@@ -5087,7 +5098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="190" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>569</v>
       </c>
@@ -5101,7 +5112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="191" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>572</v>
       </c>
@@ -5115,7 +5126,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="192" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>575</v>
       </c>
@@ -5129,7 +5140,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="193" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>578</v>
       </c>
@@ -5143,7 +5154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="194" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>581</v>
       </c>
@@ -5157,7 +5168,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="195" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>584</v>
       </c>
@@ -5171,7 +5182,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="196" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>587</v>
       </c>
@@ -5186,14 +5197,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D196" xr:uid="{F0B1C968-BD7A-47B1-B2B0-F423785F7DB9}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Turkey"/>
-        <filter val="Turkmenistan"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D196" xr:uid="{F0B1C968-BD7A-47B1-B2B0-F423785F7DB9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -5201,19 +5205,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{030FD0AA-FF69-4EA8-83A4-6C7B552075D1}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="N57" sqref="N57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>590</v>
       </c>
@@ -5221,7 +5225,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>592</v>
       </c>
@@ -5229,7 +5233,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>593</v>
       </c>
@@ -5237,7 +5241,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>594</v>
       </c>
@@ -5245,7 +5249,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>595</v>
       </c>
@@ -5253,7 +5257,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>596</v>
       </c>
@@ -5261,7 +5265,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>597</v>
       </c>
@@ -5269,7 +5273,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>598</v>
       </c>
@@ -5277,7 +5281,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>599</v>
       </c>
@@ -5285,7 +5289,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>600</v>
       </c>
@@ -5293,7 +5297,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>601</v>
       </c>
@@ -5301,7 +5305,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>602</v>
       </c>
@@ -5309,7 +5313,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>603</v>
       </c>
@@ -5317,7 +5321,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>604</v>
       </c>
@@ -5325,7 +5329,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>605</v>
       </c>
@@ -5333,7 +5337,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>606</v>
       </c>
@@ -5341,7 +5345,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>607</v>
       </c>
@@ -5349,7 +5353,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>608</v>
       </c>
@@ -5357,7 +5361,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>609</v>
       </c>
@@ -5365,7 +5369,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>610</v>
       </c>
@@ -5373,7 +5377,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>611</v>
       </c>
@@ -5381,7 +5385,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>612</v>
       </c>
@@ -5389,7 +5393,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>613</v>
       </c>
@@ -5397,7 +5401,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>614</v>
       </c>
@@ -5405,7 +5409,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>615</v>
       </c>
@@ -5413,7 +5417,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>616</v>
       </c>
@@ -5421,7 +5425,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>617</v>
       </c>
@@ -5429,7 +5433,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>618</v>
       </c>
@@ -5437,7 +5441,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>619</v>
       </c>
@@ -5445,7 +5449,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>620</v>
       </c>
@@ -5453,7 +5457,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>621</v>
       </c>
@@ -5461,7 +5465,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>622</v>
       </c>
@@ -5469,7 +5473,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>623</v>
       </c>
@@ -5477,7 +5481,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>624</v>
       </c>
@@ -5485,7 +5489,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>625</v>
       </c>
@@ -5493,7 +5497,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>626</v>
       </c>
@@ -5501,7 +5505,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>627</v>
       </c>
@@ -5509,7 +5513,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>628</v>
       </c>
@@ -5517,7 +5521,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>629</v>
       </c>
@@ -5525,7 +5529,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>630</v>
       </c>
@@ -5533,7 +5537,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>632</v>
       </c>
@@ -5541,7 +5545,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>633</v>
       </c>
@@ -5549,7 +5553,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>634</v>
       </c>
@@ -5557,7 +5561,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>635</v>
       </c>
@@ -5565,7 +5569,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>636</v>
       </c>
@@ -5573,7 +5577,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>637</v>
       </c>
@@ -5581,7 +5585,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>638</v>
       </c>
@@ -5589,7 +5593,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>639</v>
       </c>
@@ -5597,7 +5601,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>640</v>
       </c>
@@ -5605,7 +5609,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>641</v>
       </c>
@@ -5613,7 +5617,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>642</v>
       </c>
@@ -5621,7 +5625,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>643</v>
       </c>
@@ -5629,7 +5633,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>644</v>
       </c>
@@ -5637,7 +5641,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>645</v>
       </c>
@@ -5645,7 +5649,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>646</v>
       </c>
@@ -5653,7 +5657,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>647</v>
       </c>
@@ -5661,7 +5665,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>649</v>
       </c>
@@ -5669,7 +5673,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>648</v>
       </c>
@@ -5677,7 +5681,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>650</v>
       </c>
@@ -5685,7 +5689,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>651</v>
       </c>
@@ -5693,7 +5697,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>652</v>
       </c>
@@ -5701,12 +5705,36 @@
         <v>394</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>653</v>
       </c>
       <c r="B62" t="s">
         <v>560</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>654</v>
+      </c>
+      <c r="B63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>655</v>
+      </c>
+      <c r="B64" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>656</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -5724,15 +5752,15 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5746,7 +5774,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -5760,7 +5788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -5774,7 +5802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -5788,7 +5816,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -5802,7 +5830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -5816,7 +5844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -5830,7 +5858,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>93</v>
       </c>
@@ -5844,7 +5872,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -5858,7 +5886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>105</v>
       </c>
@@ -5872,7 +5900,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>108</v>
       </c>
@@ -5886,7 +5914,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>120</v>
       </c>
@@ -5900,7 +5928,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>123</v>
       </c>
@@ -5914,7 +5942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>129</v>
       </c>
@@ -5928,7 +5956,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -5942,7 +5970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>155</v>
       </c>
@@ -5956,7 +5984,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -5970,7 +5998,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>167</v>
       </c>
@@ -5984,7 +6012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>170</v>
       </c>
@@ -5998,7 +6026,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>176</v>
       </c>
@@ -6012,7 +6040,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>179</v>
       </c>
@@ -6026,7 +6054,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>191</v>
       </c>
@@ -6040,7 +6068,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>194</v>
       </c>
@@ -6054,7 +6082,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -6068,7 +6096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -6082,7 +6110,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>218</v>
       </c>
@@ -6096,7 +6124,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>272</v>
       </c>
@@ -6110,7 +6138,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>293</v>
       </c>
@@ -6124,7 +6152,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>296</v>
       </c>
@@ -6138,7 +6166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>299</v>
       </c>
@@ -6152,7 +6180,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>311</v>
       </c>
@@ -6166,7 +6194,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>314</v>
       </c>
@@ -6181,7 +6209,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>323</v>
       </c>
@@ -6196,7 +6224,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>332</v>
       </c>
@@ -6211,7 +6239,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>335</v>
       </c>
@@ -6226,7 +6254,7 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>355</v>
       </c>
@@ -6241,7 +6269,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>358</v>
       </c>
@@ -6256,7 +6284,7 @@
       </c>
       <c r="F37" s="1"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>364</v>
       </c>
@@ -6271,7 +6299,7 @@
       </c>
       <c r="F38" s="1"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>382</v>
       </c>
@@ -6286,7 +6314,7 @@
       </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>385</v>
       </c>
@@ -6301,7 +6329,7 @@
       </c>
       <c r="F40" s="1"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>436</v>
       </c>
@@ -6316,7 +6344,7 @@
       </c>
       <c r="F41" s="1"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>450</v>
       </c>
@@ -6330,7 +6358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>456</v>
       </c>
@@ -6344,7 +6372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>462</v>
       </c>
@@ -6358,7 +6386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>465</v>
       </c>
@@ -6372,7 +6400,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>479</v>
       </c>
@@ -6386,7 +6414,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>482</v>
       </c>
@@ -6400,7 +6428,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>488</v>
       </c>
@@ -6414,7 +6442,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>503</v>
       </c>
@@ -6428,7 +6456,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>521</v>
       </c>
@@ -6442,7 +6470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>530</v>
       </c>
@@ -6456,7 +6484,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>539</v>
       </c>
@@ -6470,7 +6498,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>551</v>
       </c>
@@ -6484,7 +6512,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>584</v>
       </c>
@@ -6498,7 +6526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>587</v>
       </c>
@@ -6532,15 +6560,15 @@
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6554,7 +6582,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -6568,7 +6596,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -6582,7 +6610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -6596,7 +6624,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -6610,7 +6638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -6624,7 +6652,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -6638,7 +6666,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -6652,7 +6680,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>96</v>
       </c>
@@ -6666,7 +6694,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>114</v>
       </c>
@@ -6680,7 +6708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>138</v>
       </c>
@@ -6694,7 +6722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>197</v>
       </c>
@@ -6708,7 +6736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>239</v>
       </c>
@@ -6722,7 +6750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>242</v>
       </c>
@@ -6736,7 +6764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>245</v>
       </c>
@@ -6750,7 +6778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>248</v>
       </c>
@@ -6764,7 +6792,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>254</v>
       </c>
@@ -6778,7 +6806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>263</v>
       </c>
@@ -6792,7 +6820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>266</v>
       </c>
@@ -6806,7 +6834,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>269</v>
       </c>
@@ -6820,7 +6848,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>278</v>
       </c>
@@ -6834,7 +6862,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>281</v>
       </c>
@@ -6848,7 +6876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>284</v>
       </c>
@@ -6862,7 +6890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>290</v>
       </c>
@@ -6876,7 +6904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>317</v>
       </c>
@@ -6891,7 +6919,7 @@
       </c>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>320</v>
       </c>
@@ -6906,7 +6934,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>349</v>
       </c>
@@ -6921,7 +6949,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>361</v>
       </c>
@@ -6936,7 +6964,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>370</v>
       </c>
@@ -6951,7 +6979,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>388</v>
       </c>
@@ -6966,7 +6994,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>397</v>
       </c>
@@ -6981,7 +7009,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>400</v>
       </c>
@@ -6996,7 +7024,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>418</v>
       </c>
@@ -7011,7 +7039,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>427</v>
       </c>
@@ -7026,7 +7054,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>453</v>
       </c>
@@ -7040,7 +7068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>468</v>
       </c>
@@ -7054,7 +7082,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>485</v>
       </c>
@@ -7068,7 +7096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>494</v>
       </c>
@@ -7082,7 +7110,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>500</v>
       </c>
@@ -7096,7 +7124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>515</v>
       </c>
@@ -7110,7 +7138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>518</v>
       </c>
@@ -7124,7 +7152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>524</v>
       </c>
@@ -7138,7 +7166,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>527</v>
       </c>
@@ -7152,7 +7180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>542</v>
       </c>
@@ -7166,7 +7194,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>545</v>
       </c>
@@ -7180,7 +7208,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>557</v>
       </c>
@@ -7194,7 +7222,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>569</v>
       </c>
@@ -7208,7 +7236,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>578</v>
       </c>
@@ -7222,7 +7250,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>581</v>
       </c>
@@ -7256,15 +7284,15 @@
       <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7278,7 +7306,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>33</v>
       </c>
@@ -7292,7 +7320,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>182</v>
       </c>
@@ -7306,7 +7334,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>275</v>
       </c>
@@ -7320,7 +7348,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>329</v>
       </c>
@@ -7335,7 +7363,7 @@
       </c>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>341</v>
       </c>
@@ -7350,7 +7378,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>367</v>
       </c>
@@ -7365,7 +7393,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>376</v>
       </c>
@@ -7380,7 +7408,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>403</v>
       </c>
@@ -7395,7 +7423,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>409</v>
       </c>
@@ -7410,7 +7438,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>445</v>
       </c>
@@ -7424,7 +7452,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>476</v>
       </c>
@@ -7438,7 +7466,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>533</v>
       </c>
@@ -7452,7 +7480,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>548</v>
       </c>
@@ -7466,7 +7494,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>572</v>
       </c>
@@ -7500,15 +7528,15 @@
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7522,7 +7550,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -7536,7 +7564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -7550,7 +7578,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -7564,7 +7592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -7578,7 +7606,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -7592,7 +7620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>72</v>
       </c>
@@ -7606,7 +7634,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -7620,7 +7648,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -7634,7 +7662,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -7648,7 +7676,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -7662,7 +7690,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>173</v>
       </c>
@@ -7676,7 +7704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>185</v>
       </c>
@@ -7690,7 +7718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>188</v>
       </c>
@@ -7704,7 +7732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>200</v>
       </c>
@@ -7718,7 +7746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>206</v>
       </c>
@@ -7732,7 +7760,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>227</v>
       </c>
@@ -7746,7 +7774,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>233</v>
       </c>
@@ -7760,7 +7788,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>236</v>
       </c>
@@ -7774,7 +7802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>251</v>
       </c>
@@ -7788,7 +7816,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>257</v>
       </c>
@@ -7802,7 +7830,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>287</v>
       </c>
@@ -7816,7 +7844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>302</v>
       </c>
@@ -7830,7 +7858,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>305</v>
       </c>
@@ -7844,7 +7872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>308</v>
       </c>
@@ -7858,7 +7886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>326</v>
       </c>
@@ -7873,7 +7901,7 @@
       </c>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>344</v>
       </c>
@@ -7888,7 +7916,7 @@
       </c>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>347</v>
       </c>
@@ -7903,7 +7931,7 @@
       </c>
       <c r="F28" s="1"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>352</v>
       </c>
@@ -7918,7 +7946,7 @@
       </c>
       <c r="F29" s="1"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>373</v>
       </c>
@@ -7933,7 +7961,7 @@
       </c>
       <c r="F30" s="1"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>391</v>
       </c>
@@ -7948,7 +7976,7 @@
       </c>
       <c r="F31" s="1"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>394</v>
       </c>
@@ -7963,7 +7991,7 @@
       </c>
       <c r="F32" s="1"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>421</v>
       </c>
@@ -7978,7 +8006,7 @@
       </c>
       <c r="F33" s="1"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>424</v>
       </c>
@@ -7993,7 +8021,7 @@
       </c>
       <c r="F34" s="1"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>430</v>
       </c>
@@ -8008,7 +8036,7 @@
       </c>
       <c r="F35" s="1"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>433</v>
       </c>
@@ -8023,7 +8051,7 @@
       </c>
       <c r="F36" s="1"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>448</v>
       </c>
@@ -8037,7 +8065,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>459</v>
       </c>
@@ -8051,7 +8079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>470</v>
       </c>
@@ -8065,7 +8093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>473</v>
       </c>
@@ -8079,7 +8107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>491</v>
       </c>
@@ -8093,7 +8121,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>509</v>
       </c>
@@ -8107,7 +8135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>512</v>
       </c>
@@ -8121,7 +8149,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>554</v>
       </c>
@@ -8135,7 +8163,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>560</v>
       </c>
@@ -8169,15 +8197,15 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8191,7 +8219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -8205,7 +8233,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -8219,7 +8247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -8233,7 +8261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>60</v>
       </c>
@@ -8247,7 +8275,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>102</v>
       </c>
@@ -8261,7 +8289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -8275,7 +8303,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -8289,7 +8317,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -8303,7 +8331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -8317,7 +8345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -8331,7 +8359,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>209</v>
       </c>
@@ -8345,7 +8373,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>212</v>
       </c>
@@ -8359,7 +8387,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>224</v>
       </c>
@@ -8373,7 +8401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -8387,7 +8415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>260</v>
       </c>
@@ -8401,7 +8429,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>338</v>
       </c>
@@ -8416,7 +8444,7 @@
       </c>
       <c r="F17" s="1"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>379</v>
       </c>
@@ -8431,7 +8459,7 @@
       </c>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>406</v>
       </c>
@@ -8446,7 +8474,7 @@
       </c>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>439</v>
       </c>
@@ -8461,7 +8489,7 @@
       </c>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>442</v>
       </c>
@@ -8475,7 +8503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>497</v>
       </c>
@@ -8489,7 +8517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>536</v>
       </c>
@@ -8503,7 +8531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>563</v>
       </c>
@@ -8533,15 +8561,15 @@
       <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -8555,7 +8583,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -8569,7 +8597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -8583,7 +8611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -8597,7 +8625,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>111</v>
       </c>
@@ -8611,7 +8639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -8625,7 +8653,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>158</v>
       </c>
@@ -8639,7 +8667,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>221</v>
       </c>
@@ -8653,7 +8681,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>412</v>
       </c>
@@ -8668,7 +8696,7 @@
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>415</v>
       </c>
@@ -8683,7 +8711,7 @@
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>506</v>
       </c>
@@ -8697,7 +8725,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>566</v>
       </c>
@@ -8711,7 +8739,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>575</v>
       </c>

</xml_diff>